<commit_message>
created db schema+ updated field descriptions
</commit_message>
<xml_diff>
--- a/fips/inid.xlsx
+++ b/fips/inid.xlsx
@@ -17,6 +17,7 @@
     <sheet name="БД" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ИНИД!$A$1:$E$72</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -29,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="133">
-  <si>
-    <t>дата приоритета или дата, с которой начинается действие прав промышленной собственности (дата начала отсчета срока действия патента)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="146">
   <si>
     <t xml:space="preserve"> Идентификация патента, свидетельства дополнительной охраны или патентного документа</t>
   </si>
@@ -412,12 +410,6 @@
     <t>Официальная публикация в формате PDF(ссылка)</t>
   </si>
   <si>
-    <t>119</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
     <t>Извещение об изменениях сведений в формате PDF(ссылка)</t>
   </si>
   <si>
@@ -428,6 +420,54 @@
   </si>
   <si>
     <t>multiple</t>
+  </si>
+  <si>
+    <t>use</t>
+  </si>
+  <si>
+    <t>прим. 11_href</t>
+  </si>
+  <si>
+    <t>Ссылка на реестр(заявка/патент)</t>
+  </si>
+  <si>
+    <t>Ссылка на реестр(заявка)</t>
+  </si>
+  <si>
+    <t>прим. 21_href</t>
+  </si>
+  <si>
+    <t>прим. 45_href</t>
+  </si>
+  <si>
+    <t>Официальная публикация патента в формате PDF(ссылка)</t>
+  </si>
+  <si>
+    <t>Официальная публикация заявки патента в формате PDF(ссылка)</t>
+  </si>
+  <si>
+    <t>прим. 43_href</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>Дата приоритета или дата, с которой начинается действие прав промышленной собственности (дата начала отсчета срока действия патента)</t>
   </si>
 </sst>
 </file>
@@ -451,12 +491,18 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -486,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -501,9 +547,11 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -547,9 +595,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -587,7 +635,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -659,7 +707,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -809,11 +857,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D69" sqref="D69"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,689 +871,879 @@
     <col min="3" max="3" width="108" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="E1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>27</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>31</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>34</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>40</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>41</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>42</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>43</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>44</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>45</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>46</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>47</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>48</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>50</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>51</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>52</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>54</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>56</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>57</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>58</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>60</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>61</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>62</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>63</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>64</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>65</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>66</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>67</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>68</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>70</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>71</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>72</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>73</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="D48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>74</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>75</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>76</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D51">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>80</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>81</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>83</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>84</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>85</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>86</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>87</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>88</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>90</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>91</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>92</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>93</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>94</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>95</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>96</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>97</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="6">
         <v>98</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B73" t="s">
+        <v>128</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B74" t="s">
+        <v>126</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E72"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
 </worksheet>
@@ -1513,10 +1751,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A21" sqref="A21:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,194 +1763,260 @@
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="C1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="D1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>72</v>
       </c>
       <c r="B11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" t="s">
         <v>102</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>103</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B18" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>118</v>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B20" s="5" t="s">
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B22" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B21" t="s">
-        <v>131</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
-        <v>201</v>
-      </c>
-      <c r="B22" t="s">
-        <v>129</v>
-      </c>
       <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
         <v>1</v>
       </c>
     </row>
@@ -1724,10 +2028,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,194 +2039,260 @@
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="C1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="D1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>72</v>
       </c>
       <c r="B11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" t="s">
         <v>102</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>103</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="B14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>122</v>
-      </c>
       <c r="B18" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>118</v>
+        <v>127</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B20" s="5" t="s">
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B22" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B21" t="s">
-        <v>131</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
-        <v>201</v>
-      </c>
-      <c r="B22" t="s">
-        <v>129</v>
-      </c>
       <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
connected to db, patent schema changes,patent html number/date split,date string  reformat to sql format
</commit_message>
<xml_diff>
--- a/fips/inid.xlsx
+++ b/fips/inid.xlsx
@@ -17,7 +17,7 @@
     <sheet name="БД" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ИНИД!$A$1:$E$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ИНИД!$A$1:$F$72</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="146">
-  <si>
-    <t xml:space="preserve"> Идентификация патента, свидетельства дополнительной охраны или патентного документа</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="152">
   <si>
     <t>Номер патента, свидетельства дополнительной охраны или патентного документа</t>
   </si>
@@ -468,6 +465,27 @@
   </si>
   <si>
     <t>Дата приоритета или дата, с которой начинается действие прав промышленной собственности (дата начала отсчета срока действия патента)</t>
+  </si>
+  <si>
+    <t>Статус патента/заявки</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>string/date</t>
+  </si>
+  <si>
+    <t>date/string/string</t>
+  </si>
+  <si>
+    <t>Идентификация патента, свидетельства дополнительной охраны или патентного документа</t>
   </si>
 </sst>
 </file>
@@ -551,7 +569,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -595,9 +613,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -635,7 +653,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -707,7 +725,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -857,893 +875,1113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="93.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="108" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="93.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="108" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" t="s">
         <v>129</v>
       </c>
-      <c r="E1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
+      <c r="B3" t="s">
+        <v>147</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
+      <c r="B4" t="s">
+        <v>147</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
+      <c r="B5" t="s">
+        <v>147</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
+      <c r="B6" t="s">
+        <v>147</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
+      <c r="B7" t="s">
+        <v>147</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>21</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>78</v>
+      <c r="B8" t="s">
+        <v>147</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
+        <v>77</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
+      <c r="B9" t="s">
+        <v>148</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>23</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
       <c r="E10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>24</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>145</v>
+      <c r="B11" t="s">
+        <v>148</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>25</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>26</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>27</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>30</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>82</v>
+      <c r="B15" t="s">
+        <v>147</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>21</v>
+        <v>81</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>31</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
+      <c r="B16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>32</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>84</v>
+      <c r="B17" t="s">
+        <v>148</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>33</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>85</v>
+      <c r="B18" t="s">
+        <v>147</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>34</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>40</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>41</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>12</v>
+      <c r="B21" t="s">
+        <v>148</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>42</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>148</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>43</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>86</v>
+      <c r="B23" t="s">
+        <v>148</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>44</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>148</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>45</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>111</v>
+      <c r="B25" t="s">
+        <v>148</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>46</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>87</v>
+      <c r="B26" t="s">
+        <v>148</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>47</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>148</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>48</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>148</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>50</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D29" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>51</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>88</v>
+      <c r="B30" t="s">
+        <v>147</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
+        <v>87</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>52</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>147</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>54</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>13</v>
+      <c r="B32" t="s">
+        <v>147</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>56</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>89</v>
+      <c r="B33" t="s">
+        <v>147</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>57</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>90</v>
+      <c r="B34" t="s">
+        <v>147</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>58</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>147</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>60</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>61</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>149</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>62</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>34</v>
+      <c r="B38" t="s">
+        <v>149</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D38" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>63</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>149</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>64</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>147</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>65</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>37</v>
+      <c r="B41" t="s">
+        <v>147</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D41" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>66</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
+        <v>149</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>67</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>149</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>68</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>147</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>70</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D45" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>71</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>91</v>
+      <c r="B46" t="s">
+        <v>147</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="E46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>72</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>58</v>
+      <c r="B47" t="s">
+        <v>147</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>73</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
+        <v>147</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
       <c r="E48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>74</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>92</v>
+      <c r="B49" t="s">
+        <v>147</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
+        <v>91</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="E49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>75</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>147</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>76</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>147</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>80</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D52" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>81</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>147</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>83</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>147</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>84</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>147</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>85</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>93</v>
+      <c r="B56" t="s">
+        <v>148</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>86</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>14</v>
+      <c r="B57" t="s">
+        <v>149</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>87</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>15</v>
+      <c r="B58" t="s">
+        <v>149</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>88</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>148</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>90</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="D60" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>91</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>148</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>92</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>149</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>93</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>149</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>94</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>148</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>95</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>147</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>96</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>147</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>97</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>150</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>98</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>16</v>
+      <c r="B68" t="s">
+        <v>147</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B69" t="s">
+        <v>147</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B70" t="s">
+        <v>147</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
+      <c r="D70" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="B70" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C70" s="1" t="s">
+      <c r="B71" t="s">
+        <v>147</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" t="s">
+        <v>147</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
+      <c r="F72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
+      <c r="B73" t="s">
+        <v>147</v>
+      </c>
+      <c r="C73" t="s">
+        <v>127</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B73" t="s">
-        <v>128</v>
-      </c>
-      <c r="C73">
-        <v>1</v>
-      </c>
-      <c r="D73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
-        <v>144</v>
-      </c>
       <c r="B74" t="s">
-        <v>126</v>
-      </c>
-      <c r="C74">
-        <v>1</v>
-      </c>
-      <c r="D74">
+        <v>147</v>
+      </c>
+      <c r="C74" t="s">
+        <v>125</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>127</v>
+      </c>
+      <c r="B75" t="s">
+        <v>147</v>
+      </c>
+      <c r="C75" t="s">
+        <v>145</v>
+      </c>
+      <c r="D75"/>
+      <c r="F75">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E72"/>
+  <autoFilter ref="A1:F72"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
 </worksheet>
@@ -1754,7 +1992,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:D22"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1765,16 +2003,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="C1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" t="s">
         <v>129</v>
-      </c>
-      <c r="D1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1782,7 +2020,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1793,7 +2031,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1804,7 +2042,7 @@
         <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1815,7 +2053,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1826,7 +2064,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1837,7 +2075,7 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1848,7 +2086,7 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1859,7 +2097,7 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1870,7 +2108,7 @@
         <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1881,7 +2119,7 @@
         <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1892,10 +2130,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1906,10 +2144,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1917,10 +2155,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1928,10 +2166,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1939,10 +2177,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1950,10 +2188,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1961,10 +2199,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1972,10 +2210,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1983,10 +2221,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1994,10 +2232,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2008,10 +2246,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2031,7 +2269,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A23" sqref="A23:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2041,16 +2279,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="C1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" t="s">
         <v>129</v>
-      </c>
-      <c r="D1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2058,7 +2296,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2069,7 +2307,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2080,7 +2318,7 @@
         <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2091,7 +2329,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2102,7 +2340,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2113,7 +2351,7 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2124,7 +2362,7 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2135,7 +2373,7 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2146,7 +2384,7 @@
         <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2157,7 +2395,7 @@
         <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2168,10 +2406,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2182,10 +2420,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2193,10 +2431,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -2204,10 +2442,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -2215,10 +2453,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2226,10 +2464,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -2237,10 +2475,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -2248,10 +2486,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -2259,10 +2497,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -2270,10 +2508,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2284,10 +2522,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C22">
         <v>1</v>

</xml_diff>

<commit_message>
append nonunique rows with @xxx suffix, all views created xlsx with power query
</commit_message>
<xml_diff>
--- a/fips/inid.xlsx
+++ b/fips/inid.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="6780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="6780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ИНИД" sheetId="1" r:id="rId1"/>
@@ -880,9 +880,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1997,8 +1997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>